<commit_message>
prototyping, OLED, UDP, DHT
</commit_message>
<xml_diff>
--- a/p5_weather_station/doc/weather_data_protocol.xlsx
+++ b/p5_weather_station/doc/weather_data_protocol.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nlao\School\RTOS\jhu_rtos\p5_weather_station\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nate\School\RTOS\jhu_rtos\p5_weather_station\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32E04442-218A-423B-8E0E-C0019051FC2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A749804D-9F1C-4171-98BB-C40F1C77571D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>Octet</t>
   </si>
@@ -51,16 +51,13 @@
     <t>TEMPERATURE FAHRENHEIT (Float32)</t>
   </si>
   <si>
-    <t>CRC-16 CHECKSUM</t>
-  </si>
-  <si>
     <t>TRAFFIC ID (0x45535057)</t>
   </si>
   <si>
-    <t>SPARE</t>
+    <t>ESP Weather Station Payload</t>
   </si>
   <si>
-    <t>ESP Weather Station Payload</t>
+    <t>SAMPLE NUMER (0..4294967295)</t>
   </si>
 </sst>
 </file>
@@ -84,7 +81,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -316,56 +313,102 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -651,417 +694,414 @@
   <dimension ref="B1:AI7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q18" sqref="Q18"/>
+      <selection activeCell="D4" sqref="D4:AI4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="35" width="3.77734375" customWidth="1"/>
+    <col min="4" max="35" width="3.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
-      <c r="N1" s="16"/>
-      <c r="O1" s="16"/>
-      <c r="P1" s="16"/>
-      <c r="Q1" s="16"/>
-      <c r="R1" s="16"/>
-      <c r="S1" s="16"/>
-      <c r="T1" s="16"/>
-      <c r="U1" s="16"/>
-      <c r="V1" s="16"/>
-      <c r="W1" s="16"/>
-      <c r="X1" s="16"/>
-      <c r="Y1" s="16"/>
-      <c r="Z1" s="16"/>
-      <c r="AA1" s="16"/>
-      <c r="AB1" s="16"/>
-      <c r="AC1" s="16"/>
-      <c r="AD1" s="16"/>
-      <c r="AE1" s="16"/>
-      <c r="AF1" s="16"/>
-      <c r="AG1" s="16"/>
-      <c r="AH1" s="16"/>
-      <c r="AI1" s="22"/>
+    <row r="1" spans="2:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
+      <c r="P1" s="12"/>
+      <c r="Q1" s="12"/>
+      <c r="R1" s="12"/>
+      <c r="S1" s="12"/>
+      <c r="T1" s="12"/>
+      <c r="U1" s="12"/>
+      <c r="V1" s="12"/>
+      <c r="W1" s="12"/>
+      <c r="X1" s="12"/>
+      <c r="Y1" s="12"/>
+      <c r="Z1" s="12"/>
+      <c r="AA1" s="12"/>
+      <c r="AB1" s="12"/>
+      <c r="AC1" s="12"/>
+      <c r="AD1" s="12"/>
+      <c r="AE1" s="12"/>
+      <c r="AF1" s="12"/>
+      <c r="AG1" s="12"/>
+      <c r="AH1" s="12"/>
+      <c r="AI1" s="13"/>
     </row>
-    <row r="2" spans="2:35" x14ac:dyDescent="0.3">
-      <c r="B2" s="19" t="s">
+    <row r="2" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="14">
         <v>0</v>
       </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3">
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15">
         <v>1</v>
       </c>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="3"/>
-      <c r="R2" s="3"/>
-      <c r="S2" s="3"/>
-      <c r="T2" s="3">
+      <c r="M2" s="15"/>
+      <c r="N2" s="15"/>
+      <c r="O2" s="15"/>
+      <c r="P2" s="15"/>
+      <c r="Q2" s="15"/>
+      <c r="R2" s="15"/>
+      <c r="S2" s="15"/>
+      <c r="T2" s="15">
         <v>2</v>
       </c>
-      <c r="U2" s="3"/>
-      <c r="V2" s="3"/>
-      <c r="W2" s="3"/>
-      <c r="X2" s="3"/>
-      <c r="Y2" s="3"/>
-      <c r="Z2" s="3"/>
-      <c r="AA2" s="3"/>
-      <c r="AB2" s="3">
+      <c r="U2" s="15"/>
+      <c r="V2" s="15"/>
+      <c r="W2" s="15"/>
+      <c r="X2" s="15"/>
+      <c r="Y2" s="15"/>
+      <c r="Z2" s="15"/>
+      <c r="AA2" s="15"/>
+      <c r="AB2" s="15">
         <v>3</v>
       </c>
-      <c r="AC2" s="3"/>
-      <c r="AD2" s="3"/>
-      <c r="AE2" s="3"/>
-      <c r="AF2" s="3"/>
-      <c r="AG2" s="3"/>
-      <c r="AH2" s="3"/>
-      <c r="AI2" s="4"/>
+      <c r="AC2" s="15"/>
+      <c r="AD2" s="15"/>
+      <c r="AE2" s="15"/>
+      <c r="AF2" s="15"/>
+      <c r="AG2" s="15"/>
+      <c r="AH2" s="15"/>
+      <c r="AI2" s="16"/>
     </row>
-    <row r="3" spans="2:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="7" t="s">
+    <row r="3" spans="2:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="2">
         <v>0</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="3">
         <f>D3+1</f>
         <v>1</v>
       </c>
-      <c r="F3" s="8">
-        <f t="shared" ref="F3:AN3" si="0">E3+1</f>
+      <c r="F3" s="3">
+        <f t="shared" ref="F3:AI3" si="0">E3+1</f>
         <v>2</v>
       </c>
-      <c r="G3" s="8">
+      <c r="G3" s="3">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="H3" s="8">
+      <c r="H3" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="I3" s="8">
+      <c r="I3" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="J3" s="8">
+      <c r="J3" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="K3" s="8">
+      <c r="K3" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="L3" s="8">
+      <c r="L3" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="M3" s="8">
+      <c r="M3" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="N3" s="8">
+      <c r="N3" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="O3" s="8">
+      <c r="O3" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="P3" s="8">
+      <c r="P3" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="Q3" s="8">
+      <c r="Q3" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="R3" s="8">
+      <c r="R3" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="S3" s="8">
+      <c r="S3" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="T3" s="8">
+      <c r="T3" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="U3" s="8">
+      <c r="U3" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="V3" s="8">
+      <c r="V3" s="3">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="W3" s="8">
+      <c r="W3" s="3">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="X3" s="8">
+      <c r="X3" s="3">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="Y3" s="8">
+      <c r="Y3" s="3">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="Z3" s="8">
+      <c r="Z3" s="3">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="AA3" s="8">
+      <c r="AA3" s="3">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="AB3" s="8">
+      <c r="AB3" s="3">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="AC3" s="8">
+      <c r="AC3" s="3">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="AD3" s="8">
+      <c r="AD3" s="3">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="AE3" s="8">
+      <c r="AE3" s="3">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="AF3" s="8">
+      <c r="AF3" s="3">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="AG3" s="8">
+      <c r="AG3" s="3">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="AH3" s="8">
+      <c r="AH3" s="3">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="AI3" s="21">
+      <c r="AI3" s="10">
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="2:35" x14ac:dyDescent="0.3">
-      <c r="B4" s="17">
+    <row r="4" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B4" s="6">
         <v>0</v>
       </c>
-      <c r="C4" s="18">
+      <c r="C4" s="7">
         <v>0</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
-      <c r="O4" s="3"/>
-      <c r="P4" s="3"/>
-      <c r="Q4" s="3"/>
-      <c r="R4" s="3"/>
-      <c r="S4" s="3"/>
-      <c r="T4" s="3"/>
-      <c r="U4" s="3"/>
-      <c r="V4" s="3"/>
-      <c r="W4" s="3"/>
-      <c r="X4" s="3"/>
-      <c r="Y4" s="3"/>
-      <c r="Z4" s="3"/>
-      <c r="AA4" s="3"/>
-      <c r="AB4" s="3"/>
-      <c r="AC4" s="3"/>
-      <c r="AD4" s="3"/>
-      <c r="AE4" s="3"/>
-      <c r="AF4" s="3"/>
-      <c r="AG4" s="3"/>
-      <c r="AH4" s="3"/>
-      <c r="AI4" s="4"/>
+      <c r="D4" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="15"/>
+      <c r="L4" s="15"/>
+      <c r="M4" s="15"/>
+      <c r="N4" s="15"/>
+      <c r="O4" s="15"/>
+      <c r="P4" s="15"/>
+      <c r="Q4" s="15"/>
+      <c r="R4" s="15"/>
+      <c r="S4" s="15"/>
+      <c r="T4" s="15"/>
+      <c r="U4" s="15"/>
+      <c r="V4" s="15"/>
+      <c r="W4" s="15"/>
+      <c r="X4" s="15"/>
+      <c r="Y4" s="15"/>
+      <c r="Z4" s="15"/>
+      <c r="AA4" s="15"/>
+      <c r="AB4" s="15"/>
+      <c r="AC4" s="15"/>
+      <c r="AD4" s="15"/>
+      <c r="AE4" s="15"/>
+      <c r="AF4" s="15"/>
+      <c r="AG4" s="15"/>
+      <c r="AH4" s="15"/>
+      <c r="AI4" s="16"/>
     </row>
-    <row r="5" spans="2:35" x14ac:dyDescent="0.3">
-      <c r="B5" s="5">
+    <row r="5" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B5" s="1">
         <v>4</v>
       </c>
-      <c r="C5" s="11">
+      <c r="C5" s="4">
         <v>32</v>
       </c>
-      <c r="D5" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
-      <c r="O5" s="1"/>
-      <c r="P5" s="1"/>
-      <c r="Q5" s="1"/>
-      <c r="R5" s="1"/>
-      <c r="S5" s="1"/>
-      <c r="T5" s="1" t="s">
+      <c r="D5" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="U5" s="1"/>
-      <c r="V5" s="1"/>
-      <c r="W5" s="1"/>
-      <c r="X5" s="1"/>
-      <c r="Y5" s="1"/>
-      <c r="Z5" s="1"/>
-      <c r="AA5" s="1"/>
-      <c r="AB5" s="1"/>
-      <c r="AC5" s="1"/>
-      <c r="AD5" s="1"/>
-      <c r="AE5" s="1"/>
-      <c r="AF5" s="1"/>
-      <c r="AG5" s="1"/>
-      <c r="AH5" s="1"/>
-      <c r="AI5" s="6"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="24"/>
+      <c r="J5" s="24"/>
+      <c r="K5" s="24"/>
+      <c r="L5" s="24"/>
+      <c r="M5" s="24"/>
+      <c r="N5" s="24"/>
+      <c r="O5" s="24"/>
+      <c r="P5" s="24"/>
+      <c r="Q5" s="24"/>
+      <c r="R5" s="24"/>
+      <c r="S5" s="24"/>
+      <c r="T5" s="24"/>
+      <c r="U5" s="24"/>
+      <c r="V5" s="24"/>
+      <c r="W5" s="24"/>
+      <c r="X5" s="24"/>
+      <c r="Y5" s="24"/>
+      <c r="Z5" s="24"/>
+      <c r="AA5" s="24"/>
+      <c r="AB5" s="24"/>
+      <c r="AC5" s="24"/>
+      <c r="AD5" s="24"/>
+      <c r="AE5" s="24"/>
+      <c r="AF5" s="24"/>
+      <c r="AG5" s="24"/>
+      <c r="AH5" s="24"/>
+      <c r="AI5" s="25"/>
     </row>
-    <row r="6" spans="2:35" x14ac:dyDescent="0.3">
-      <c r="B6" s="5">
+    <row r="6" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B6" s="1">
         <v>8</v>
       </c>
-      <c r="C6" s="11">
+      <c r="C6" s="4">
         <v>64</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D6" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
-      <c r="O6" s="1"/>
-      <c r="P6" s="1"/>
-      <c r="Q6" s="1"/>
-      <c r="R6" s="1"/>
-      <c r="S6" s="1"/>
-      <c r="T6" s="1"/>
-      <c r="U6" s="1"/>
-      <c r="V6" s="1"/>
-      <c r="W6" s="1"/>
-      <c r="X6" s="1"/>
-      <c r="Y6" s="1"/>
-      <c r="Z6" s="1"/>
-      <c r="AA6" s="1"/>
-      <c r="AB6" s="1"/>
-      <c r="AC6" s="1"/>
-      <c r="AD6" s="1"/>
-      <c r="AE6" s="1"/>
-      <c r="AF6" s="1"/>
-      <c r="AG6" s="1"/>
-      <c r="AH6" s="1"/>
-      <c r="AI6" s="6"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="21"/>
+      <c r="I6" s="21"/>
+      <c r="J6" s="21"/>
+      <c r="K6" s="21"/>
+      <c r="L6" s="21"/>
+      <c r="M6" s="21"/>
+      <c r="N6" s="21"/>
+      <c r="O6" s="21"/>
+      <c r="P6" s="21"/>
+      <c r="Q6" s="21"/>
+      <c r="R6" s="21"/>
+      <c r="S6" s="21"/>
+      <c r="T6" s="21"/>
+      <c r="U6" s="21"/>
+      <c r="V6" s="21"/>
+      <c r="W6" s="21"/>
+      <c r="X6" s="21"/>
+      <c r="Y6" s="21"/>
+      <c r="Z6" s="21"/>
+      <c r="AA6" s="21"/>
+      <c r="AB6" s="21"/>
+      <c r="AC6" s="21"/>
+      <c r="AD6" s="21"/>
+      <c r="AE6" s="21"/>
+      <c r="AF6" s="21"/>
+      <c r="AG6" s="21"/>
+      <c r="AH6" s="21"/>
+      <c r="AI6" s="22"/>
     </row>
-    <row r="7" spans="2:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="7">
+    <row r="7" spans="2:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="2">
         <v>12</v>
       </c>
-      <c r="C7" s="12">
+      <c r="C7" s="5">
         <v>96</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="D7" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
-      <c r="K7" s="9"/>
-      <c r="L7" s="9"/>
-      <c r="M7" s="9"/>
-      <c r="N7" s="9"/>
-      <c r="O7" s="9"/>
-      <c r="P7" s="9"/>
-      <c r="Q7" s="9"/>
-      <c r="R7" s="9"/>
-      <c r="S7" s="9"/>
-      <c r="T7" s="9"/>
-      <c r="U7" s="9"/>
-      <c r="V7" s="9"/>
-      <c r="W7" s="9"/>
-      <c r="X7" s="9"/>
-      <c r="Y7" s="9"/>
-      <c r="Z7" s="9"/>
-      <c r="AA7" s="9"/>
-      <c r="AB7" s="9"/>
-      <c r="AC7" s="9"/>
-      <c r="AD7" s="9"/>
-      <c r="AE7" s="9"/>
-      <c r="AF7" s="9"/>
-      <c r="AG7" s="9"/>
-      <c r="AH7" s="9"/>
-      <c r="AI7" s="10"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="18"/>
+      <c r="M7" s="18"/>
+      <c r="N7" s="18"/>
+      <c r="O7" s="18"/>
+      <c r="P7" s="18"/>
+      <c r="Q7" s="18"/>
+      <c r="R7" s="18"/>
+      <c r="S7" s="18"/>
+      <c r="T7" s="18"/>
+      <c r="U7" s="18"/>
+      <c r="V7" s="18"/>
+      <c r="W7" s="18"/>
+      <c r="X7" s="18"/>
+      <c r="Y7" s="18"/>
+      <c r="Z7" s="18"/>
+      <c r="AA7" s="18"/>
+      <c r="AB7" s="18"/>
+      <c r="AC7" s="18"/>
+      <c r="AD7" s="18"/>
+      <c r="AE7" s="18"/>
+      <c r="AF7" s="18"/>
+      <c r="AG7" s="18"/>
+      <c r="AH7" s="18"/>
+      <c r="AI7" s="19"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="9">
+    <mergeCell ref="D7:AI7"/>
+    <mergeCell ref="D6:AI6"/>
+    <mergeCell ref="D4:AI4"/>
+    <mergeCell ref="D5:AI5"/>
     <mergeCell ref="B1:AI1"/>
     <mergeCell ref="D2:K2"/>
     <mergeCell ref="L2:S2"/>
     <mergeCell ref="T2:AA2"/>
     <mergeCell ref="AB2:AI2"/>
-    <mergeCell ref="D7:AI7"/>
-    <mergeCell ref="D6:AI6"/>
-    <mergeCell ref="D5:S5"/>
-    <mergeCell ref="D4:AI4"/>
-    <mergeCell ref="T5:AI5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>